<commit_message>
Final del Recorrido, Verificar
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/AL.xlsx
+++ b/OYM/_DocumentosComunes/AL.xlsx
@@ -773,8 +773,8 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A190" sqref="A36:XFD190"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -943,7 +943,9 @@
       <c r="F4" s="6">
         <v>20</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6">
+        <v>40</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3">
         <v>1</v>
@@ -956,11 +958,11 @@
       </c>
       <c r="N4">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1017,13 +1019,14 @@
         <v>10</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="F6" s="6">
         <v>20</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6">
+        <v>50</v>
+      </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
@@ -1044,11 +1047,11 @@
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>40.5</v>
+        <v>91</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>90.5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1066,13 +1069,14 @@
         <v>10</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="6">
         <v>18</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6">
+        <v>39</v>
+      </c>
       <c r="H7" s="3">
         <v>1</v>
       </c>
@@ -1089,11 +1093,11 @@
       <c r="M7" s="9"/>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>30.5</v>
+        <v>70</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>80.5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1148,13 +1152,14 @@
         <v>9</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="6">
         <v>16</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6">
+        <v>42</v>
+      </c>
       <c r="H9" s="3">
         <v>1</v>
       </c>
@@ -1169,11 +1174,11 @@
       <c r="M9" s="9"/>
       <c r="N9">
         <f t="shared" si="2"/>
-        <v>27.5</v>
+        <v>70</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>77.5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1343,13 +1348,14 @@
         <v>10</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="F14" s="6">
         <v>20</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6">
+        <v>45</v>
+      </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
@@ -1370,11 +1376,11 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>37.5</v>
+        <v>85</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>87.5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1388,17 +1394,17 @@
         <v>33</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F15" s="6">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="G15" s="6">
+        <v>40</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
         <v>1</v>
@@ -1411,11 +1417,11 @@
       <c r="M15" s="9"/>
       <c r="N15">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1575,13 +1581,14 @@
         <v>10</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F20" s="6">
         <v>20</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="6">
+        <v>50</v>
+      </c>
       <c r="H20" s="3">
         <v>1</v>
       </c>
@@ -1600,11 +1607,11 @@
       </c>
       <c r="N20">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="O20">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1622,13 +1629,14 @@
         <v>10</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>10</v>
       </c>
       <c r="F21" s="6">
         <v>20</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="6">
+        <v>50</v>
+      </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
@@ -1647,11 +1655,11 @@
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>34.5</v>
+        <v>90</v>
       </c>
       <c r="O21">
         <f t="shared" si="3"/>
-        <v>84.5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1774,13 +1782,14 @@
         <v>10</v>
       </c>
       <c r="E25" s="6">
-        <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="F25" s="6">
         <v>20</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="G25" s="6">
+        <v>50</v>
+      </c>
       <c r="H25" s="3">
         <v>1</v>
       </c>
@@ -1801,11 +1810,11 @@
       </c>
       <c r="N25">
         <f t="shared" si="2"/>
-        <v>40.5</v>
+        <v>90</v>
       </c>
       <c r="O25">
         <f t="shared" si="3"/>
-        <v>90.5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,13 +1832,14 @@
         <v>10</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="F26" s="6">
         <v>20</v>
       </c>
-      <c r="G26" s="6"/>
+      <c r="G26" s="6">
+        <v>50</v>
+      </c>
       <c r="H26" s="3">
         <v>1</v>
       </c>
@@ -1848,11 +1858,11 @@
       </c>
       <c r="N26">
         <f t="shared" si="2"/>
-        <v>36.5</v>
+        <v>90</v>
       </c>
       <c r="O26">
         <f t="shared" si="3"/>
-        <v>86.5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1948,13 +1958,14 @@
         <v>10</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="6">
         <v>19</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6">
+        <v>40</v>
+      </c>
       <c r="H29" s="3">
         <v>1</v>
       </c>
@@ -1969,11 +1980,11 @@
       <c r="M29" s="9"/>
       <c r="N29">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="O29">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2073,13 +2084,14 @@
         <v>10</v>
       </c>
       <c r="E32" s="6">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F32" s="6">
         <v>20</v>
       </c>
-      <c r="G32" s="6"/>
+      <c r="G32" s="6">
+        <v>45</v>
+      </c>
       <c r="H32" s="3">
         <v>1</v>
       </c>
@@ -2100,11 +2112,11 @@
       </c>
       <c r="N32">
         <f t="shared" si="2"/>
-        <v>34.5</v>
+        <v>80</v>
       </c>
       <c r="O32">
         <f t="shared" si="3"/>
-        <v>84.5</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2122,13 +2134,14 @@
         <v>10</v>
       </c>
       <c r="E33" s="6">
-        <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="F33" s="6">
         <v>20</v>
       </c>
-      <c r="G33" s="6"/>
+      <c r="G33" s="6">
+        <v>50</v>
+      </c>
       <c r="H33" s="3">
         <v>1</v>
       </c>
@@ -2149,11 +2162,11 @@
       </c>
       <c r="N33">
         <f t="shared" si="2"/>
-        <v>40.5</v>
+        <v>91</v>
       </c>
       <c r="O33">
         <f t="shared" si="3"/>
-        <v>90.5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,8 +2180,7 @@
         <v>71</v>
       </c>
       <c r="D34" s="6">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E34" s="6">
         <f t="shared" si="1"/>
@@ -2177,7 +2189,9 @@
       <c r="F34" s="6">
         <v>10</v>
       </c>
-      <c r="G34" s="6"/>
+      <c r="G34" s="6">
+        <v>50</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -2186,11 +2200,11 @@
       <c r="M34" s="9"/>
       <c r="N34">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="O34">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2208,13 +2222,14 @@
         <v>10</v>
       </c>
       <c r="E35" s="6">
-        <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>20</v>
       </c>
       <c r="F35" s="6">
         <v>20</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="6">
+        <v>50</v>
+      </c>
       <c r="H35" s="3">
         <v>1</v>
       </c>
@@ -2235,11 +2250,11 @@
       </c>
       <c r="N35">
         <f t="shared" si="2"/>
-        <v>40.5</v>
+        <v>100</v>
       </c>
       <c r="O35">
         <f t="shared" si="3"/>
-        <v>90.5</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>